<commit_message>
All Character's Face Uploaded
大きさ調整しないとあかんかもだけどひとまず
</commit_message>
<xml_diff>
--- a/Assets/End/resource/data_resource.xlsx
+++ b/Assets/End/resource/data_resource.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="145">
   <si>
     <t>data_resource</t>
   </si>
@@ -950,10 +950,6 @@
     <t>http://game-icons.net/</t>
   </si>
   <si>
-    <t>ここからとってきてる</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>skill</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1027,10 +1023,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>title_white</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>title_bg</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1059,28 +1051,35 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>英語フォント(アセットストアから)→quadrangle</t>
-    <rPh sb="0" eb="2">
-      <t>エイゴ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイトルフォントはこれ→https://fontmeme.com/fonts/judas-priest-font/</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日本語フォント→http://sawarabi-fonts.osdn.jp/</t>
+    <t>http://roughsketch.en-grey.com/</t>
+  </si>
+  <si>
+    <t>https://soundeffect-lab.info/</t>
+  </si>
+  <si>
+    <t>http://sawarabi-fonts.osdn.jp/</t>
+  </si>
+  <si>
+    <t>さわらびフォント</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://fontmeme.com/fonts/judas-priest-font/</t>
+  </si>
+  <si>
+    <t>judas priestフォント</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>game-icons</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>三日月アルペジオ</t>
     <rPh sb="0" eb="3">
-      <t>ニホンゴ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>http://roughsketch.en-grey.com/</t>
-  </si>
-  <si>
-    <t>https://soundeffect-lab.info/</t>
+      <t>ミカヅキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>効果音ラボ</t>
@@ -1090,45 +1089,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>顔グラ</t>
-    <rPh sb="0" eb="1">
-      <t>カオ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>http://sawarabi-fonts.osdn.jp/</t>
-  </si>
-  <si>
-    <t>さわらびフォント</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://fontmeme.com/fonts/judas-priest-font/</t>
-  </si>
-  <si>
-    <t>judas priestフォント</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>game-icons</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>三日月アルペジオ</t>
-    <rPh sb="0" eb="3">
-      <t>ミカヅキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>効果音ラボ</t>
-    <rPh sb="0" eb="3">
-      <t>コウカオン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>http://www.vita-chi.net/sozai1.htm</t>
   </si>
   <si>
@@ -1163,6 +1123,13 @@
   </si>
   <si>
     <t>誰そ彼亭</t>
+  </si>
+  <si>
+    <t>http://sorejanai.blog.shinobi.jp/</t>
+  </si>
+  <si>
+    <t>そういうんじゃないから</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1607,7 +1574,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1655,7 +1622,7 @@
     </row>
     <row r="11" spans="1:7" ht="16.2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
@@ -1663,20 +1630,20 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="G12" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>110</v>
@@ -1684,44 +1651,54 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G15" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="G18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G21" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G22" s="3" t="s">
-        <v>148</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G25" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1913,7 +1890,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2037,16 +2014,6 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>134</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2055,11 +2022,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2113,7 +2078,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
@@ -2121,61 +2086,40 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>125</v>
-      </c>
-    </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>131</v>
-      </c>
+      <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>130</v>
-      </c>
+      <c r="A17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>132</v>
-      </c>
+      <c r="A18" s="3"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2187,7 +2131,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2374,22 +2318,12 @@
     </row>
     <row r="28" spans="1:2" ht="16.2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2408,42 +2342,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>